<commit_message>
first time added to repository
</commit_message>
<xml_diff>
--- a/xcelfiles/demoqaReg.xlsx
+++ b/xcelfiles/demoqaReg.xlsx
@@ -17,10 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
-  <si>
-    <t/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>First Name</t>
   </si>
@@ -74,13 +71,106 @@
   </si>
   <si>
     <t>user@gmail.com</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>Mill</t>
+  </si>
+  <si>
+    <t>AdactinHotel BOOKING DETAILS</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>PassWord</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Melbourne</t>
+  </si>
+  <si>
+    <t>password@12345</t>
+  </si>
+  <si>
+    <t>Hotels</t>
+  </si>
+  <si>
+    <t>Hotel Sunshine</t>
+  </si>
+  <si>
+    <t>RoomType</t>
+  </si>
+  <si>
+    <t>Super Deluxe</t>
+  </si>
+  <si>
+    <t>No.of Rooms</t>
+  </si>
+  <si>
+    <t>DateIn</t>
+  </si>
+  <si>
+    <t>Dateout</t>
+  </si>
+  <si>
+    <t>AdultperRoom</t>
+  </si>
+  <si>
+    <t>ChildrenPerRoom</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> USA</t>
+  </si>
+  <si>
+    <t>CreditDardTpe</t>
+  </si>
+  <si>
+    <t>MAST</t>
+  </si>
+  <si>
+    <t>MonthText</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>yearVAlue</t>
+  </si>
+  <si>
+    <t>Cvv</t>
+  </si>
+  <si>
+    <t>user94446</t>
+  </si>
+  <si>
+    <t>CreditCardNo</t>
+  </si>
+  <si>
+    <t>BookingOrderNo = :7X5YKTBMOP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +185,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,9 +214,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -466,88 +570,231 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C3">
         <v>9770695332</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" t="s">
+        <v>40</v>
+      </c>
+      <c r="P10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>44</v>
+      </c>
+      <c r="R10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="3">
+        <v>4</v>
+      </c>
+      <c r="G11" s="4">
+        <v>44553</v>
+      </c>
+      <c r="H11" s="4">
+        <v>44555</v>
+      </c>
+      <c r="I11" s="5">
+        <v>2</v>
+      </c>
+      <c r="J11" s="5">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" t="s">
+        <v>39</v>
+      </c>
+      <c r="N11">
+        <v>9876543209876540</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q11">
+        <v>2022</v>
+      </c>
+      <c r="R11">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -555,7 +802,9 @@
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
     <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B11" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>